<commit_message>
modified Map Fps Sdb
</commit_message>
<xml_diff>
--- a/Data Files/Excel_Files/TestCaseData.xlsx
+++ b/Data Files/Excel_Files/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545" tabRatio="793" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545" tabRatio="793" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Activity_Controlor_API" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="399">
   <si>
     <t>owner</t>
   </si>
@@ -210,9 +210,6 @@
     <t>statusCode</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>initActivity</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>fpskeySequence</t>
   </si>
   <si>
-    <t>pqr</t>
-  </si>
-  <si>
     <t>efskey</t>
   </si>
   <si>
@@ -387,21 +381,6 @@
     <t>txn</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>mapType</t>
   </si>
   <si>
@@ -600,9 +579,6 @@
     <t>blockSize</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>SDB</t>
   </si>
   <si>
@@ -981,9 +957,6 @@
     <t>SCR</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>10018</t>
   </si>
   <si>
@@ -1234,6 +1207,30 @@
   </si>
   <si>
     <t>0000001255 0000001255 0000001255 0000001255 0000001255 0000001255 0000007630 0000007628</t>
+  </si>
+  <si>
+    <t>dgAction</t>
+  </si>
+  <si>
+    <t>highUseIndicator</t>
+  </si>
+  <si>
+    <t>extendedAttribute</t>
+  </si>
+  <si>
+    <t>dynamicTxnCode</t>
+  </si>
+  <si>
+    <t>defExtendedAttribute</t>
+  </si>
+  <si>
+    <t>txnAttribute</t>
+  </si>
+  <si>
+    <t>nonPemMapIndicator</t>
+  </si>
+  <si>
+    <t>logDbType</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1671,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>8</v>
@@ -1683,16 +1680,16 @@
         <v>9</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1703,13 +1700,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1719,10 +1716,10 @@
       <c r="K2" s="4"/>
       <c r="L2" s="2"/>
       <c r="M2" s="4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1734,25 +1731,25 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1780,7 +1777,7 @@
         <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>29</v>
@@ -1789,16 +1786,16 @@
         <v>30</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1811,7 +1808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
@@ -1833,125 +1830,125 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="G1" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>244</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1974,61 +1971,61 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="O4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="P4" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2052,7 +2049,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2062,7 +2059,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2103,7 +2100,7 @@
         <v>18</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>5</v>
@@ -2120,16 +2117,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -2138,7 +2135,7 @@
         <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2146,7 +2143,7 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -2155,7 +2152,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
@@ -2218,19 +2215,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2248,10 +2245,10 @@
         <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>47</v>
@@ -2263,7 +2260,7 @@
         <v>49</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2276,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,7 +2287,7 @@
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
@@ -2301,7 +2298,7 @@
     <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2334,52 +2331,52 @@
         <v>57</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="W1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -2387,43 +2384,45 @@
         <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>21</v>
@@ -2432,11 +2431,13 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="V2" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="W2" s="2"/>
       <c r="X2" s="4"/>
       <c r="Y2" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2451,14 +2452,14 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -2466,25 +2467,25 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="V3" s="2" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="Y3" s="2"/>
     </row>
@@ -2493,76 +2494,76 @@
         <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="N4" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="O4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="S4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="T4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="X4" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="Y4" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2575,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,15 +2593,17 @@
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>43</v>
@@ -2615,106 +2618,108 @@
         <v>8</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2728,74 +2733,72 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
-        <v>315</v>
-      </c>
+      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="L4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="P4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="R4" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="S4" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2831,75 +2834,75 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>1</v>
@@ -2908,18 +2911,18 @@
         <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2937,46 +2940,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2989,8 +2992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,100 +3009,100 @@
     <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>187</v>
-      </c>
       <c r="N1" s="9" t="s">
-        <v>188</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3117,46 +3120,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3186,7 +3189,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>17</v>
@@ -3198,28 +3201,28 @@
         <v>54</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>5</v>
@@ -3227,34 +3230,34 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>21</v>
@@ -3266,7 +3269,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3280,48 +3283,48 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3368,115 +3371,115 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="G1" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="T1" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="P1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z1" s="9" t="s">
         <v>344</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
@@ -3494,7 +3497,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>1</v>
@@ -3509,7 +3512,7 @@
         <v>1</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>1</v>
@@ -3526,7 +3529,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3535,14 +3538,14 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -3560,82 +3563,82 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="L4" s="2">
         <v>56</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="Z4" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>